<commit_message>
Correct CT scanner names in DCM_Partners.xlsx etc
</commit_message>
<xml_diff>
--- a/GN/Data/DCM_Partners.xlsx
+++ b/GN/Data/DCM_Partners.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hoffman\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hoffman\GN\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86506A07-9793-4AB1-88F4-3646B91A6BA0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1947DE26-1674-4A18-81C0-C1C5ABE1B4B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{381DDAB4-8499-413C-B235-A2766B27323F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="506">
   <si>
     <t>PET</t>
   </si>
@@ -1552,156 +1552,6 @@
   </si>
   <si>
     <t>D:\Hoffman\_WMIC\Hoffman_Skull_2014_06_09\6x5mm_CTAC_3x21_128_z2-7_4mm (AC)\Frame6</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_Manchester\CNMNC_Hoffman_PET_2014_05_30_DRAFT\STD CT Brain\9002</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_Manchester\CNMNC_Hoffman_PET_2014_05_30_DRAFT\STD CT Brain\9003</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_Manchester\CNMNC_Hoffman_PET_2014_05_30_DRAFT\STD CT Brain\9004</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_Manchester\CNMNC_Hoffman_PET_2014_05_30_DRAFT\STD CT Brain\9005</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_Manchester\CNMNC_Hoffman_PET_2014_05_30_DRAFT\STD CT Brain\9006</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_Manchester\CNMNC_Hoffman_PET_2014_05_30_DRAFT\STD CT Brain\9007</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_Manchester\CNMNC_Hoffman_PET_2014_05_30_DRAFT\STD CT Brain\9008</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_RoyalSurrey\Skull\AC_CT_BRAIN_TOUR_0013</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_RoyalSurrey\Skull\AC_CT_BRAIN_TOUR_0014</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_RoyalSurrey\Skull\AC_CT_BRAIN_TOUR_0015</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_RoyalSurrey\Skull\AC_CT_BRAIN_TOUR_0016</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_RoyalSurrey\Skull\AC_CT_BRAIN_TOUR_0017</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_RoyalSurrey\Skull\AC_CT_BRAIN_TOUR_0018</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_RoyalSurrey\Skull\AC_CT_BRAIN_TOUR_0019</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_RoyalSurrey\Skull\AC_CT_BRAIN_TOUR_0020</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_RoyalSurrey\Skull\AC_CT_BRAIN_TOUR_0021</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_RoyalSurrey\Skull\AC_CT_BRAIN_TOUR_0022</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_RoyalSurrey\NoSkull\AC_CT_BRAIN_TOUR_0011</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_RoyalSurrey\NoSkull\AC_CT_BRAIN_TOUR_0012</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_RoyalSurrey\NoSkull\AC_CT_BRAIN_TOUR_0013</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_RoyalSurrey\NoSkull\AC_CT_BRAIN_TOUR_0014</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_RoyalSurrey\NoSkull\AC_CT_BRAIN_TOUR_0015</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_RoyalSurrey\NoSkull\AC_CT_BRAIN_TOUR_0016</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_RoyalSurrey\NoSkull\AC_CT_BRAIN_TOUR_0017</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_RoyalSurrey\NoSkull\AC_CT_BRAIN_TOUR_0018</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_RoyalSurrey\NoSkull\AC_CT_BRAIN_TOUR_0019</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_RoyalSurrey\NoSkull\AC_CT_BRAIN_TOUR_0020</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_RoyalSurrey\NoSkull\AC_CT_BRAIN_TOUR_0021</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_Sheffield\CT_noskull\S51</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_Sheffield\CT_noskull\S52</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_Sheffield\CT_noskull\S53</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_Sheffield\CT_noskull\S54</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_Sheffield\CT_noskull\S55</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_Sheffield\CT_noskull\S56</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_Sheffield\CT_noskull\S57</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_Sheffield\CT_noskull\S58</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_Sheffield\CT_noskull\S59</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_Sheffield\CT_noskull\S60</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_Sheffield\CT_noskull\S61</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_Sheffield\CT_withskull\S31</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_Sheffield\CT_withskull\S32</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_Sheffield\CT_withskull\S33</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_Sheffield\CT_withskull\S34</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_Sheffield\CT_withskull\S35</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_Sheffield\CT_withskull\S36</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_Sheffield\CT_withskull\S37</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_Sheffield\CT_withskull\S38</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_Sheffield\CT_withskull\S39</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_Sheffield\CT_withskull\S40</t>
-  </si>
-  <si>
-    <t>D:\Hoffman\CT_AllCentres\_Sheffield\CT_withskull\S41</t>
   </si>
 </sst>
 </file>
@@ -2061,8 +1911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29FC6EEC-E0F0-4AAB-8EF0-DE3DFC8E217F}">
   <dimension ref="A1:B464"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="84" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A441" zoomScale="84" workbookViewId="0">
+      <selection activeCell="B356" sqref="B356"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4156,7 +4006,7 @@
         <v>302</v>
       </c>
       <c r="B261" t="s">
-        <v>506</v>
+        <v>23</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.3">
@@ -4164,7 +4014,7 @@
         <v>303</v>
       </c>
       <c r="B262" t="s">
-        <v>507</v>
+        <v>23</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.3">
@@ -4172,7 +4022,7 @@
         <v>304</v>
       </c>
       <c r="B263" t="s">
-        <v>508</v>
+        <v>23</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.3">
@@ -4180,7 +4030,7 @@
         <v>305</v>
       </c>
       <c r="B264" t="s">
-        <v>509</v>
+        <v>23</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.3">
@@ -4188,7 +4038,7 @@
         <v>306</v>
       </c>
       <c r="B265" t="s">
-        <v>510</v>
+        <v>23</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.3">
@@ -4196,7 +4046,7 @@
         <v>307</v>
       </c>
       <c r="B266" t="s">
-        <v>511</v>
+        <v>23</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.3">
@@ -4204,7 +4054,7 @@
         <v>308</v>
       </c>
       <c r="B267" t="s">
-        <v>512</v>
+        <v>23</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.3">
@@ -4556,7 +4406,7 @@
         <v>352</v>
       </c>
       <c r="B311" t="s">
-        <v>523</v>
+        <v>27</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.3">
@@ -4564,7 +4414,7 @@
         <v>353</v>
       </c>
       <c r="B312" t="s">
-        <v>524</v>
+        <v>27</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.3">
@@ -4572,7 +4422,7 @@
         <v>354</v>
       </c>
       <c r="B313" t="s">
-        <v>525</v>
+        <v>27</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.3">
@@ -4580,7 +4430,7 @@
         <v>355</v>
       </c>
       <c r="B314" t="s">
-        <v>526</v>
+        <v>27</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.3">
@@ -4588,7 +4438,7 @@
         <v>356</v>
       </c>
       <c r="B315" t="s">
-        <v>527</v>
+        <v>27</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.3">
@@ -4596,7 +4446,7 @@
         <v>357</v>
       </c>
       <c r="B316" t="s">
-        <v>528</v>
+        <v>27</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.3">
@@ -4604,7 +4454,7 @@
         <v>358</v>
       </c>
       <c r="B317" t="s">
-        <v>529</v>
+        <v>27</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.3">
@@ -4612,7 +4462,7 @@
         <v>359</v>
       </c>
       <c r="B318" t="s">
-        <v>530</v>
+        <v>27</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.3">
@@ -4620,7 +4470,7 @@
         <v>360</v>
       </c>
       <c r="B319" t="s">
-        <v>531</v>
+        <v>27</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.3">
@@ -4628,7 +4478,7 @@
         <v>361</v>
       </c>
       <c r="B320" t="s">
-        <v>532</v>
+        <v>27</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.3">
@@ -4636,7 +4486,7 @@
         <v>362</v>
       </c>
       <c r="B321" t="s">
-        <v>533</v>
+        <v>27</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.3">
@@ -4652,7 +4502,7 @@
         <v>364</v>
       </c>
       <c r="B323" t="s">
-        <v>513</v>
+        <v>28</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.3">
@@ -4660,7 +4510,7 @@
         <v>365</v>
       </c>
       <c r="B324" t="s">
-        <v>514</v>
+        <v>28</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.3">
@@ -4668,7 +4518,7 @@
         <v>366</v>
       </c>
       <c r="B325" t="s">
-        <v>515</v>
+        <v>28</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.3">
@@ -4676,7 +4526,7 @@
         <v>367</v>
       </c>
       <c r="B326" t="s">
-        <v>516</v>
+        <v>28</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.3">
@@ -4684,7 +4534,7 @@
         <v>368</v>
       </c>
       <c r="B327" t="s">
-        <v>517</v>
+        <v>28</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.3">
@@ -4692,7 +4542,7 @@
         <v>369</v>
       </c>
       <c r="B328" t="s">
-        <v>518</v>
+        <v>28</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.3">
@@ -4700,7 +4550,7 @@
         <v>370</v>
       </c>
       <c r="B329" t="s">
-        <v>519</v>
+        <v>28</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.3">
@@ -4708,7 +4558,7 @@
         <v>371</v>
       </c>
       <c r="B330" t="s">
-        <v>520</v>
+        <v>28</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.3">
@@ -4716,7 +4566,7 @@
         <v>372</v>
       </c>
       <c r="B331" t="s">
-        <v>521</v>
+        <v>28</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.3">
@@ -4724,7 +4574,7 @@
         <v>373</v>
       </c>
       <c r="B332" t="s">
-        <v>522</v>
+        <v>28</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.3">
@@ -4740,7 +4590,7 @@
         <v>375</v>
       </c>
       <c r="B334" t="s">
-        <v>534</v>
+        <v>29</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.3">
@@ -4748,7 +4598,7 @@
         <v>376</v>
       </c>
       <c r="B335" t="s">
-        <v>535</v>
+        <v>29</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.3">
@@ -4756,7 +4606,7 @@
         <v>377</v>
       </c>
       <c r="B336" t="s">
-        <v>536</v>
+        <v>29</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.3">
@@ -4764,7 +4614,7 @@
         <v>378</v>
       </c>
       <c r="B337" t="s">
-        <v>537</v>
+        <v>29</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.3">
@@ -4772,7 +4622,7 @@
         <v>379</v>
       </c>
       <c r="B338" t="s">
-        <v>538</v>
+        <v>29</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.3">
@@ -4780,7 +4630,7 @@
         <v>380</v>
       </c>
       <c r="B339" t="s">
-        <v>539</v>
+        <v>29</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.3">
@@ -4788,7 +4638,7 @@
         <v>381</v>
       </c>
       <c r="B340" t="s">
-        <v>540</v>
+        <v>29</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.3">
@@ -4796,7 +4646,7 @@
         <v>382</v>
       </c>
       <c r="B341" t="s">
-        <v>541</v>
+        <v>29</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.3">
@@ -4804,7 +4654,7 @@
         <v>383</v>
       </c>
       <c r="B342" t="s">
-        <v>542</v>
+        <v>29</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.3">
@@ -4812,7 +4662,7 @@
         <v>384</v>
       </c>
       <c r="B343" t="s">
-        <v>543</v>
+        <v>29</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.3">
@@ -4820,7 +4670,7 @@
         <v>385</v>
       </c>
       <c r="B344" t="s">
-        <v>544</v>
+        <v>29</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.3">
@@ -4836,7 +4686,7 @@
         <v>387</v>
       </c>
       <c r="B346" t="s">
-        <v>545</v>
+        <v>30</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.3">
@@ -4844,7 +4694,7 @@
         <v>388</v>
       </c>
       <c r="B347" t="s">
-        <v>546</v>
+        <v>30</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.3">
@@ -4852,7 +4702,7 @@
         <v>389</v>
       </c>
       <c r="B348" t="s">
-        <v>547</v>
+        <v>30</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.3">
@@ -4860,7 +4710,7 @@
         <v>390</v>
       </c>
       <c r="B349" t="s">
-        <v>548</v>
+        <v>30</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.3">
@@ -4868,7 +4718,7 @@
         <v>391</v>
       </c>
       <c r="B350" t="s">
-        <v>549</v>
+        <v>30</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.3">
@@ -4876,7 +4726,7 @@
         <v>392</v>
       </c>
       <c r="B351" t="s">
-        <v>550</v>
+        <v>30</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.3">
@@ -4884,7 +4734,7 @@
         <v>393</v>
       </c>
       <c r="B352" t="s">
-        <v>551</v>
+        <v>30</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.3">
@@ -4892,7 +4742,7 @@
         <v>394</v>
       </c>
       <c r="B353" t="s">
-        <v>552</v>
+        <v>30</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.3">
@@ -4900,7 +4750,7 @@
         <v>395</v>
       </c>
       <c r="B354" t="s">
-        <v>553</v>
+        <v>30</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.3">
@@ -4908,7 +4758,7 @@
         <v>396</v>
       </c>
       <c r="B355" t="s">
-        <v>554</v>
+        <v>30</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.3">
@@ -4916,7 +4766,7 @@
         <v>397</v>
       </c>
       <c r="B356" t="s">
-        <v>555</v>
+        <v>30</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>